<commit_message>
Everything but merge and comment quick
</commit_message>
<xml_diff>
--- a/Lab7-Timings.xlsx
+++ b/Lab7-Timings.xlsx
@@ -531,6 +531,12 @@
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.9618</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.9102</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -540,11 +546,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>37500.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>75000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>150000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,11 +633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2138774864"/>
-        <c:axId val="2145527808"/>
+        <c:axId val="2139989664"/>
+        <c:axId val="2139992896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2138774864"/>
+        <c:axId val="2139989664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,12 +694,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2145527808"/>
+        <c:crossAx val="2139992896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145527808"/>
+        <c:axId val="2139992896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +755,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138774864"/>
+        <c:crossAx val="2139989664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1684,7 +1693,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1848,13 +1857,22 @@
       <c r="B9">
         <v>4</v>
       </c>
+      <c r="C9">
+        <v>37500</v>
+      </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>75000</v>
+      </c>
+      <c r="E9">
+        <v>15.9618</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>150000</v>
+      </c>
+      <c r="G9">
+        <v>64.910200000000003</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Code Finished with comments, finishing excel
</commit_message>
<xml_diff>
--- a/Lab7-Timings.xlsx
+++ b/Lab7-Timings.xlsx
@@ -254,10 +254,10 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.64692</c:v>
+                  <c:v>8.28044</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.2637</c:v>
+                  <c:v>21.7112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,13 +269,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.8E7</c:v>
+                  <c:v>1.0E8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.76E8</c:v>
+                  <c:v>2.0E8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.52E8</c:v>
+                  <c:v>4.0E8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -327,6 +327,12 @@
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.9224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.5538</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -336,11 +342,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.135E6</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>2.27E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>4.54E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,6 +475,12 @@
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.3771</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.4522</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -475,11 +490,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>31000.0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>62000.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>124000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -605,6 +623,12 @@
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.3662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.0894</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -614,11 +638,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.908E6</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>3.816E6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>7.632E6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -633,11 +660,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2139989664"/>
-        <c:axId val="2139992896"/>
+        <c:axId val="2095455312"/>
+        <c:axId val="2095452080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2139989664"/>
+        <c:axId val="2095455312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,12 +721,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139992896"/>
+        <c:crossAx val="2095452080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2139992896"/>
+        <c:axId val="2095452080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2139989664"/>
+        <c:crossAx val="2095455312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1693,7 +1720,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,21 +1791,21 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>88000000</v>
+        <v>100000000</v>
       </c>
       <c r="D5">
         <f>2*C5</f>
-        <v>176000000</v>
+        <v>200000000</v>
       </c>
       <c r="E5">
-        <v>8.6469199999999997</v>
+        <v>8.2804400000000005</v>
       </c>
       <c r="F5">
         <f>2*D5</f>
-        <v>352000000</v>
+        <v>400000000</v>
       </c>
       <c r="G5">
-        <v>22.2637</v>
+        <v>21.711200000000002</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
@@ -1791,13 +1818,22 @@
       <c r="B6">
         <v>4</v>
       </c>
+      <c r="C6">
+        <v>1135000</v>
+      </c>
       <c r="D6">
         <f t="shared" ref="D6:D10" si="0">2*C6</f>
-        <v>0</v>
+        <v>2270000</v>
+      </c>
+      <c r="E6">
+        <v>15.9224</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F10" si="1">2*D6</f>
-        <v>0</v>
+        <v>4540000</v>
+      </c>
+      <c r="G6">
+        <v>62.553800000000003</v>
       </c>
       <c r="H6" t="s">
         <v>14</v>
@@ -1838,13 +1874,22 @@
       <c r="B8">
         <v>4</v>
       </c>
+      <c r="C8">
+        <v>31000</v>
+      </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62000</v>
+      </c>
+      <c r="E8">
+        <v>16.377099999999999</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>124000</v>
+      </c>
+      <c r="G8">
+        <v>65.452200000000005</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
@@ -1885,13 +1930,22 @@
       <c r="B10">
         <v>4</v>
       </c>
+      <c r="C10">
+        <v>1908000</v>
+      </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3816000</v>
+      </c>
+      <c r="E10">
+        <v>8.3661999999999992</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7632000</v>
+      </c>
+      <c r="G10">
+        <v>17.089400000000001</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>

</xml_diff>